<commit_message>
add edit entity parameters component
</commit_message>
<xml_diff>
--- a/CollectionDataLoader/backend/upload.xlsx
+++ b/CollectionDataLoader/backend/upload.xlsx
@@ -15,14 +15,14 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'204363 (14-2)'!$A$1:$H$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'204461 (16-2)'!$A$1:$H$736</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Defenetion!$D$1:$D$76</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Defenetion!$D$1:$D$77</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11311" uniqueCount="2654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11314" uniqueCount="2656">
   <si>
     <t>Case ID</t>
   </si>
@@ -7665,9 +7665,6 @@
     <t>DWH_CUSTOMER</t>
   </si>
   <si>
-    <t>P1</t>
-  </si>
-  <si>
     <t>Column</t>
   </si>
   <si>
@@ -7713,9 +7710,6 @@
     <t>Parameters</t>
   </si>
   <si>
-    <t>$p1</t>
-  </si>
-  <si>
     <t>dd/mm/yyyy</t>
   </si>
   <si>
@@ -7830,13 +7824,171 @@
     <t>CUST_CLUSTER</t>
   </si>
   <si>
-    <t>select customer_id from customer_all c  where C.CUSTCODE=$p1</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
     <t>select CUSTCODE from customer_all where  CUSTOMER_ID = $key</t>
+  </si>
+  <si>
+    <t>select BILLCYCLE
+from customer_all where custcode='5.46429'</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>3G Lenient</t>
+  </si>
+  <si>
+    <t>3G Normal</t>
+  </si>
+  <si>
+    <t>Cmbentry7</t>
+  </si>
+  <si>
+    <t>Cmbentry2</t>
+  </si>
+  <si>
+    <t>AVL consumer</t>
+  </si>
+  <si>
+    <t>select COMBO07
+from INFO_CUST_COMBO where customer_id=$key</t>
+  </si>
+  <si>
+    <t>Premium</t>
+  </si>
+  <si>
+    <t>Primary</t>
+  </si>
+  <si>
+    <t>Platinum</t>
+  </si>
+  <si>
+    <t>Intermediate</t>
+  </si>
+  <si>
+    <t>Strategic</t>
+  </si>
+  <si>
+    <t>PCSP</t>
+  </si>
+  <si>
+    <t>Value 4</t>
+  </si>
+  <si>
+    <t>select   case when prgcode  in(1,7) then 1
+         else 2  end
+from customer_all where custcode='5.46429'</t>
+  </si>
+  <si>
+    <t>SELECT nvl(sum(ohopnamt_gl),0)
+ FROM orderhdr_all
+ WHERE orderhdr_all.customer_id =  $key
+ AND ohstatus = 'IN'
+ AND ohopnamt_gl &gt; 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT min(OHENTDATE)
+ FROM orderhdr_all
+ WHERE orderhdr_all.customer_id =  $key
+ AND ohstatus = 'IN'
+ AND ohopnamt_gl &gt; 0  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SELECT count(*)
+ FROM orderhdr_all
+ WHERE orderhdr_all.customer_id = $key
+ AND ohstatus = 'IN'
+ AND ohopnamt_gl &gt; 0 </t>
+  </si>
+  <si>
+    <t>Cairo</t>
+  </si>
+  <si>
+    <t>select  CC.CCTN_AREA ||' ' ||CC.CCTN from CCONTACT_ALL cc where CC.CCBILL='X' and CC.CUSTOMER_ID =$key</t>
+  </si>
+  <si>
+    <t>select  CC.CCTN2_AREA ||' ' ||CC.CCTN2 from CCONTACT_ALL cc where CC.CCBILL='X' and CC.CUSTOMER_ID =$key</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> select sum (nvl(CACHKAMT_GL,0))
+ from cashreceipts_all cr
+ where cr.customer_id  = $key and cr.CATYPE in (10,12)</t>
+  </si>
+  <si>
+    <t>select CSACTIVATED from customer_all where customer_id=$key</t>
+  </si>
+  <si>
+    <t>select PRGNAME from customer_all c , PRICEGROUP_ALL pg
+  where customer_id=$key
+        and C.PRGCODE = PG.PRGCODE</t>
+  </si>
+  <si>
+    <t>select CC.CCSTATE from CCONTACT_ALL cc where CC.CCBILL='X' and CC.CUSTOMER_ID = $key</t>
+  </si>
+  <si>
+    <t>select text15 from  info_cust_text  where CUSTOMER_ID =$key</t>
+  </si>
+  <si>
+    <t>ISP-Premium</t>
+  </si>
+  <si>
+    <t>ISP-Intermediate</t>
+  </si>
+  <si>
+    <t>ISP-Strategic</t>
+  </si>
+  <si>
+    <t>ISP-Primary</t>
+  </si>
+  <si>
+    <t>Double</t>
+  </si>
+  <si>
+    <t>1/3/2018</t>
+  </si>
+  <si>
+    <t>5.46429</t>
+  </si>
+  <si>
+    <t>cust_code</t>
+  </si>
+  <si>
+    <t>select customer_id from customer_all c  where C.CUSTCODE=$cust_code</t>
+  </si>
+  <si>
+    <t>$cust_code</t>
   </si>
   <si>
     <t xml:space="preserve">select count(con.co_id)
@@ -7853,7 +8005,7 @@
 (
 select  c.CUSTOMER_ID
 from customer_all c
-start with C.CUSTCODE =$p1
+start with C.CUSTCODE =$cust_code
 CONNECT BY  PRIOR C.CUSTOMER_ID =  C.CUSTOMER_ID_HIGH 
             and  nvl(C.PAYMNTRESP,'N') &lt;&gt; 'X'
 ) </t>
@@ -7873,7 +8025,7 @@
 (
 select  c.CUSTOMER_ID
 from customer_all c
-start with C.CUSTCODE = $p1
+start with C.CUSTCODE = $cust_code
 CONNECT BY  PRIOR C.CUSTOMER_ID =  C.CUSTOMER_ID_HIGH 
             and  nvl(C.PAYMNTRESP,'N') &lt;&gt; 'X'
 )  </t>
@@ -7888,7 +8040,7 @@
 (
 select  c.CUSTOMER_ID
 from customer_all c
-start with C.CUSTCODE = $p1
+start with C.CUSTCODE = $cust_code
 CONNECT BY  PRIOR C.CUSTOMER_ID =  C.CUSTOMER_ID_HIGH 
             and  nvl(C.PAYMNTRESP,'N') &lt;&gt; 'X'
 ) </t>
@@ -7904,153 +8056,10 @@
 (
 select  c.CUSTOMER_ID
 from customer_all c
-start with C.CUSTCODE = $p1
+start with C.CUSTCODE = $cust_code
 CONNECT BY  PRIOR C.CUSTOMER_ID =  C.CUSTOMER_ID_HIGH 
             and  nvl(C.PAYMNTRESP,'N') &lt;&gt; 'X'
 ) </t>
-  </si>
-  <si>
-    <t>select BILLCYCLE
-from customer_all where custcode='5.46429'</t>
-  </si>
-  <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>09</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>08</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>07</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>3G Lenient</t>
-  </si>
-  <si>
-    <t>3G Normal</t>
-  </si>
-  <si>
-    <t>Cmbentry7</t>
-  </si>
-  <si>
-    <t>Cmbentry2</t>
-  </si>
-  <si>
-    <t>AVL consumer</t>
-  </si>
-  <si>
-    <t>select COMBO07
-from INFO_CUST_COMBO where customer_id=$key</t>
-  </si>
-  <si>
-    <t>Premium</t>
-  </si>
-  <si>
-    <t>Primary</t>
-  </si>
-  <si>
-    <t>Platinum</t>
-  </si>
-  <si>
-    <t>Intermediate</t>
-  </si>
-  <si>
-    <t>Strategic</t>
-  </si>
-  <si>
-    <t>PCSP</t>
-  </si>
-  <si>
-    <t>Value 4</t>
-  </si>
-  <si>
-    <t>select   case when prgcode  in(1,7) then 1
-         else 2  end
-from customer_all where custcode='5.46429'</t>
-  </si>
-  <si>
-    <t>SELECT nvl(sum(ohopnamt_gl),0)
- FROM orderhdr_all
- WHERE orderhdr_all.customer_id =  $key
- AND ohstatus = 'IN'
- AND ohopnamt_gl &gt; 0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SELECT min(OHENTDATE)
- FROM orderhdr_all
- WHERE orderhdr_all.customer_id =  $key
- AND ohstatus = 'IN'
- AND ohopnamt_gl &gt; 0  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SELECT count(*)
- FROM orderhdr_all
- WHERE orderhdr_all.customer_id = $key
- AND ohstatus = 'IN'
- AND ohopnamt_gl &gt; 0 </t>
-  </si>
-  <si>
-    <t>Cairo</t>
-  </si>
-  <si>
-    <t>select  CC.CCTN_AREA ||' ' ||CC.CCTN from CCONTACT_ALL cc where CC.CCBILL='X' and CC.CUSTOMER_ID =$key</t>
-  </si>
-  <si>
-    <t>select  CC.CCTN2_AREA ||' ' ||CC.CCTN2 from CCONTACT_ALL cc where CC.CCBILL='X' and CC.CUSTOMER_ID =$key</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> select sum (nvl(CACHKAMT_GL,0))
- from cashreceipts_all cr
- where cr.customer_id  = $key and cr.CATYPE in (10,12)</t>
-  </si>
-  <si>
-    <t>select CSACTIVATED from customer_all where customer_id=$key</t>
-  </si>
-  <si>
-    <t>select PRGNAME from customer_all c , PRICEGROUP_ALL pg
-  where customer_id=$key
-        and C.PRGCODE = PG.PRGCODE</t>
-  </si>
-  <si>
-    <t>select CC.CCSTATE from CCONTACT_ALL cc where CC.CCBILL='X' and CC.CUSTOMER_ID = $key</t>
-  </si>
-  <si>
-    <t>select text15 from  info_cust_text  where CUSTOMER_ID =$key</t>
-  </si>
-  <si>
-    <t>ISP-Premium</t>
-  </si>
-  <si>
-    <t>ISP-Intermediate</t>
-  </si>
-  <si>
-    <t>ISP-Strategic</t>
-  </si>
-  <si>
-    <t>ISP-Primary</t>
   </si>
   <si>
     <t xml:space="preserve">select count(con.co_id)
@@ -8072,19 +8081,16 @@
 (
 select  c.CUSTOMER_ID
 from customer_all c
-start with C.CUSTCODE = $p1
+start with C.CUSTCODE = $cust_code
 CONNECT BY  PRIOR C.CUSTOMER_ID =  C.CUSTOMER_ID_HIGH 
             and  nvl(C.PAYMNTRESP,'N') &lt;&gt; 'X'
 ) </t>
   </si>
   <si>
-    <t>Double</t>
-  </si>
-  <si>
-    <t>1/3/2018</t>
-  </si>
-  <si>
-    <t>5.46429</t>
+    <t>cust_name</t>
+  </si>
+  <si>
+    <t>ddd</t>
   </si>
 </sst>
 </file>
@@ -8745,13 +8751,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -8786,13 +8792,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -8827,13 +8833,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -8868,13 +8874,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -8909,13 +8915,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -8950,13 +8956,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -8991,13 +8997,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -9032,13 +9038,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -9073,13 +9079,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -9114,13 +9120,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -9155,13 +9161,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -9196,13 +9202,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -9237,13 +9243,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -9278,13 +9284,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -9319,13 +9325,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -9360,13 +9366,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -9401,13 +9407,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -9442,13 +9448,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -9483,13 +9489,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -9524,13 +9530,13 @@
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
           <xdr:colOff>304800</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>21</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -57089,10 +57095,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I76"/>
+  <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57116,10 +57122,10 @@
         <v>2546</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>2566</v>
+        <v>2564</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>2552</v>
+        <v>2551</v>
       </c>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
@@ -57129,16 +57135,16 @@
     </row>
     <row r="2" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>2562</v>
+        <v>2561</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>2550</v>
+        <v>2549</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>2560</v>
+        <v>2559</v>
       </c>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
@@ -57148,13 +57154,13 @@
     </row>
     <row r="3" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>2547</v>
+        <v>2646</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>2653</v>
+        <v>2645</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
@@ -57163,230 +57169,232 @@
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
+        <v>2654</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>2655</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>2558</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>2547</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>2560</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>2549</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>2554</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>2559</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>2548</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>2561</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>2550</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>2555</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>2560</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>2549</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>2551</v>
-      </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>2543</v>
-      </c>
-      <c r="B5" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7" t="s">
-        <v>2557</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7" t="s">
-        <v>2553</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>2602</v>
       </c>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
     </row>
-    <row r="6" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>2567</v>
+        <v>2543</v>
       </c>
       <c r="B6" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>2563</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C6" s="7"/>
       <c r="D6" s="7" t="s">
-        <v>2559</v>
+        <v>2556</v>
       </c>
       <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="10"/>
+      <c r="F6" s="7" t="s">
+        <v>2552</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>2647</v>
+      </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>2568</v>
+        <v>2565</v>
       </c>
       <c r="B7" s="7" t="b">
         <v>0</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>2603</v>
+        <v>2648</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="G7" s="10"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>2569</v>
+        <v>2566</v>
       </c>
       <c r="B8" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="C8" s="7"/>
+      <c r="C8" s="7" t="s">
+        <v>2600</v>
+      </c>
       <c r="D8" s="7" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
       <c r="E8" s="7"/>
-      <c r="F8" s="7" t="s">
-        <v>2553</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>2604</v>
-      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>2570</v>
+        <v>2567</v>
       </c>
       <c r="B9" s="7" t="b">
         <v>0</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7" t="s">
-        <v>2557</v>
+        <v>2558</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>2605</v>
+        <v>2601</v>
       </c>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" ht="405" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>2571</v>
+        <v>2568</v>
       </c>
       <c r="B10" s="7" t="b">
         <v>0</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="7" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>2606</v>
+        <v>2649</v>
       </c>
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:9" s="5" customFormat="1" ht="240" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="405" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>2572</v>
+        <v>2569</v>
       </c>
       <c r="B11" s="7" t="b">
         <v>0</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="7" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>2607</v>
+        <v>2650</v>
       </c>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:9" s="5" customFormat="1" ht="255" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="5" customFormat="1" ht="240" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>2573</v>
+        <v>2570</v>
       </c>
       <c r="B12" s="7" t="b">
         <v>0</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>2608</v>
+        <v>2651</v>
       </c>
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="5" customFormat="1" ht="255" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>2574</v>
+        <v>2571</v>
       </c>
       <c r="B13" s="7" t="b">
         <v>0</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>2609</v>
+        <v>2652</v>
       </c>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>2572</v>
+      </c>
+      <c r="B14" s="7" t="b">
+        <v>0</v>
+      </c>
       <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+      <c r="D14" s="7" t="s">
+        <v>2556</v>
+      </c>
       <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="7" t="s">
-        <v>2610</v>
-      </c>
-      <c r="I14" s="7">
-        <v>1</v>
-      </c>
+      <c r="F14" s="7" t="s">
+        <v>2552</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>2602</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
     </row>
     <row r="15" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
@@ -57397,10 +57405,10 @@
       <c r="F15" s="7"/>
       <c r="G15" s="9"/>
       <c r="H15" s="7" t="s">
-        <v>2611</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>2612</v>
+        <v>2603</v>
+      </c>
+      <c r="I15" s="7">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57412,10 +57420,10 @@
       <c r="F16" s="7"/>
       <c r="G16" s="9"/>
       <c r="H16" s="7" t="s">
-        <v>2613</v>
+        <v>2604</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>2614</v>
+        <v>2605</v>
       </c>
     </row>
     <row r="17" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57427,10 +57435,10 @@
       <c r="F17" s="7"/>
       <c r="G17" s="9"/>
       <c r="H17" s="7" t="s">
-        <v>2615</v>
+        <v>2606</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>2616</v>
+        <v>2607</v>
       </c>
     </row>
     <row r="18" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57442,10 +57450,10 @@
       <c r="F18" s="7"/>
       <c r="G18" s="9"/>
       <c r="H18" s="7" t="s">
-        <v>2617</v>
+        <v>2608</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>2618</v>
+        <v>2609</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57457,43 +57465,39 @@
       <c r="F19" s="7"/>
       <c r="G19" s="9"/>
       <c r="H19" s="7" t="s">
-        <v>2619</v>
+        <v>2610</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>2620</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>2575</v>
-      </c>
-      <c r="B20" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="C20" s="7">
-        <v>2</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>2557</v>
-      </c>
+        <v>2611</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="7" t="s">
+        <v>2612</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>2613</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>2576</v>
+        <v>2573</v>
       </c>
       <c r="B21" s="7" t="b">
         <v>0</v>
       </c>
       <c r="C21" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -57501,41 +57505,45 @@
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>2577</v>
+        <v>2574</v>
       </c>
       <c r="B22" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="C22" s="7"/>
+      <c r="C22" s="7">
+        <v>1</v>
+      </c>
       <c r="D22" s="7" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="E22" s="7"/>
-      <c r="F22" s="7" t="s">
-        <v>2553</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>2626</v>
-      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="7"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
+    <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>2575</v>
+      </c>
+      <c r="B23" s="7" t="b">
+        <v>0</v>
+      </c>
       <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
+      <c r="D23" s="7" t="s">
+        <v>2556</v>
+      </c>
       <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="7" t="s">
-        <v>2621</v>
-      </c>
-      <c r="I23" s="7">
-        <v>87438</v>
-      </c>
+      <c r="F23" s="7" t="s">
+        <v>2552</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>2619</v>
+      </c>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
     </row>
     <row r="24" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
@@ -57546,10 +57554,10 @@
       <c r="F24" s="7"/>
       <c r="G24" s="9"/>
       <c r="H24" s="7" t="s">
-        <v>2622</v>
+        <v>2614</v>
       </c>
       <c r="I24" s="7">
-        <v>87439</v>
+        <v>87438</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57560,9 +57568,11 @@
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="7"/>
+      <c r="H25" s="7" t="s">
+        <v>2615</v>
+      </c>
       <c r="I25" s="7">
-        <v>-1</v>
+        <v>87439</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57573,11 +57583,9 @@
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="9"/>
-      <c r="H26" s="7" t="s">
-        <v>1166</v>
-      </c>
+      <c r="H26" s="7"/>
       <c r="I26" s="7">
-        <v>14914</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="27" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57589,10 +57597,10 @@
       <c r="F27" s="7"/>
       <c r="G27" s="9"/>
       <c r="H27" s="7" t="s">
-        <v>985</v>
+        <v>1166</v>
       </c>
       <c r="I27" s="7">
-        <v>14920</v>
+        <v>14914</v>
       </c>
     </row>
     <row r="28" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57604,10 +57612,10 @@
       <c r="F28" s="7"/>
       <c r="G28" s="9"/>
       <c r="H28" s="7" t="s">
-        <v>11</v>
+        <v>985</v>
       </c>
       <c r="I28" s="7">
-        <v>14917</v>
+        <v>14920</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57619,10 +57627,10 @@
       <c r="F29" s="7"/>
       <c r="G29" s="9"/>
       <c r="H29" s="7" t="s">
-        <v>2623</v>
+        <v>11</v>
       </c>
       <c r="I29" s="7">
-        <v>16032</v>
+        <v>14917</v>
       </c>
     </row>
     <row r="30" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57634,10 +57642,10 @@
       <c r="F30" s="7"/>
       <c r="G30" s="9"/>
       <c r="H30" s="7" t="s">
-        <v>2624</v>
+        <v>2616</v>
       </c>
       <c r="I30" s="7">
-        <v>14912</v>
+        <v>16032</v>
       </c>
     </row>
     <row r="31" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57649,10 +57657,10 @@
       <c r="F31" s="7"/>
       <c r="G31" s="9"/>
       <c r="H31" s="7" t="s">
-        <v>18</v>
+        <v>2617</v>
       </c>
       <c r="I31" s="7">
-        <v>88956</v>
+        <v>14912</v>
       </c>
     </row>
     <row r="32" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57664,10 +57672,10 @@
       <c r="F32" s="7"/>
       <c r="G32" s="9"/>
       <c r="H32" s="7" t="s">
-        <v>873</v>
+        <v>18</v>
       </c>
       <c r="I32" s="7">
-        <v>99900</v>
+        <v>88956</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57679,10 +57687,10 @@
       <c r="F33" s="7"/>
       <c r="G33" s="9"/>
       <c r="H33" s="7" t="s">
-        <v>1134</v>
+        <v>873</v>
       </c>
       <c r="I33" s="7">
-        <v>83772</v>
+        <v>99900</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57694,10 +57702,10 @@
       <c r="F34" s="7"/>
       <c r="G34" s="9"/>
       <c r="H34" s="7" t="s">
-        <v>112</v>
+        <v>1134</v>
       </c>
       <c r="I34" s="7">
-        <v>14913</v>
+        <v>83772</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57709,10 +57717,10 @@
       <c r="F35" s="7"/>
       <c r="G35" s="9"/>
       <c r="H35" s="7" t="s">
-        <v>517</v>
+        <v>112</v>
       </c>
       <c r="I35" s="7">
-        <v>91669</v>
+        <v>14913</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57724,10 +57732,10 @@
       <c r="F36" s="7"/>
       <c r="G36" s="9"/>
       <c r="H36" s="7" t="s">
-        <v>2625</v>
+        <v>517</v>
       </c>
       <c r="I36" s="7">
-        <v>106400</v>
+        <v>91669</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57739,45 +57747,47 @@
       <c r="F37" s="7"/>
       <c r="G37" s="9"/>
       <c r="H37" s="7" t="s">
+        <v>2618</v>
+      </c>
+      <c r="I37" s="7">
+        <v>106400</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="7" t="s">
         <v>835</v>
       </c>
-      <c r="I37" s="7">
+      <c r="I38" s="7">
         <v>211423</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
-        <v>2578</v>
-      </c>
-      <c r="B38" s="7" t="b">
+    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>2576</v>
+      </c>
+      <c r="B39" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7" t="s">
-        <v>2557</v>
-      </c>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7" t="s">
-        <v>2553</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>2626</v>
-      </c>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-    </row>
-    <row r="39" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
       <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
+      <c r="D39" s="7" t="s">
+        <v>2556</v>
+      </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="9"/>
+      <c r="F39" s="7" t="s">
+        <v>2552</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>2619</v>
+      </c>
       <c r="H39" s="7"/>
-      <c r="I39" s="7">
-        <v>-2</v>
-      </c>
+      <c r="I39" s="7"/>
     </row>
     <row r="40" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
@@ -57787,11 +57797,9 @@
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="9"/>
-      <c r="H40" s="7" t="s">
-        <v>2627</v>
-      </c>
+      <c r="H40" s="7"/>
       <c r="I40" s="7">
-        <v>12784</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57803,10 +57811,10 @@
       <c r="F41" s="7"/>
       <c r="G41" s="9"/>
       <c r="H41" s="7" t="s">
-        <v>2628</v>
+        <v>2620</v>
       </c>
       <c r="I41" s="7">
-        <v>12785</v>
+        <v>12784</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57818,10 +57826,10 @@
       <c r="F42" s="7"/>
       <c r="G42" s="9"/>
       <c r="H42" s="7" t="s">
-        <v>2629</v>
+        <v>2621</v>
       </c>
       <c r="I42" s="7">
-        <v>21271</v>
+        <v>12785</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57833,10 +57841,10 @@
       <c r="F43" s="7"/>
       <c r="G43" s="9"/>
       <c r="H43" s="7" t="s">
-        <v>2630</v>
+        <v>2622</v>
       </c>
       <c r="I43" s="7">
-        <v>12202</v>
+        <v>21271</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57848,10 +57856,10 @@
       <c r="F44" s="7"/>
       <c r="G44" s="9"/>
       <c r="H44" s="7" t="s">
-        <v>2631</v>
+        <v>2623</v>
       </c>
       <c r="I44" s="7">
-        <v>12926</v>
+        <v>12202</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57863,10 +57871,10 @@
       <c r="F45" s="7"/>
       <c r="G45" s="9"/>
       <c r="H45" s="7" t="s">
-        <v>2632</v>
+        <v>2624</v>
       </c>
       <c r="I45" s="7">
-        <v>12778</v>
+        <v>12926</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57878,10 +57886,10 @@
       <c r="F46" s="7"/>
       <c r="G46" s="9"/>
       <c r="H46" s="7" t="s">
-        <v>2633</v>
+        <v>2625</v>
       </c>
       <c r="I46" s="7">
-        <v>12965</v>
+        <v>12778</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -57892,172 +57900,168 @@
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
       <c r="G47" s="9"/>
-      <c r="H47" s="7">
+      <c r="H47" s="7" t="s">
+        <v>2626</v>
+      </c>
+      <c r="I47" s="7">
+        <v>12965</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="7">
         <v>1</v>
       </c>
-      <c r="I47" s="7">
+      <c r="I48" s="7">
         <v>5126</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
-        <v>2579</v>
-      </c>
-      <c r="B48" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7" t="s">
-        <v>2557</v>
-      </c>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7" t="s">
-        <v>2553</v>
-      </c>
-      <c r="G48" s="9" t="s">
-        <v>2634</v>
-      </c>
-      <c r="H48" s="7"/>
-      <c r="I48" s="7"/>
-    </row>
-    <row r="49" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>2580</v>
+        <v>2577</v>
       </c>
       <c r="B49" s="7" t="b">
         <v>0</v>
       </c>
       <c r="C49" s="7"/>
       <c r="D49" s="7" t="s">
-        <v>2651</v>
+        <v>2556</v>
       </c>
       <c r="E49" s="7"/>
       <c r="F49" s="7" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="G49" s="9" t="s">
-        <v>2635</v>
+        <v>2627</v>
       </c>
       <c r="H49" s="7"/>
       <c r="I49" s="7"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>2581</v>
+        <v>2578</v>
       </c>
       <c r="B50" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="C50" s="7">
-        <v>0</v>
-      </c>
+      <c r="C50" s="7"/>
       <c r="D50" s="7" t="s">
-        <v>2651</v>
+        <v>2643</v>
       </c>
       <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
+      <c r="F50" s="7" t="s">
+        <v>2552</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>2628</v>
+      </c>
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
     </row>
-    <row r="51" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>2582</v>
+        <v>2579</v>
       </c>
       <c r="B51" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="C51" s="7"/>
+      <c r="C51" s="7">
+        <v>0</v>
+      </c>
       <c r="D51" s="7" t="s">
-        <v>2556</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>2564</v>
-      </c>
-      <c r="F51" s="7" t="s">
-        <v>2553</v>
-      </c>
-      <c r="G51" s="9" t="s">
-        <v>2636</v>
-      </c>
+        <v>2643</v>
+      </c>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>2583</v>
+        <v>2580</v>
       </c>
       <c r="B52" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="C52" s="7" t="s">
-        <v>14</v>
-      </c>
+      <c r="C52" s="7"/>
       <c r="D52" s="7" t="s">
-        <v>2559</v>
-      </c>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
+        <v>2555</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>2562</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>2552</v>
+      </c>
+      <c r="G52" s="9" t="s">
+        <v>2629</v>
+      </c>
       <c r="H52" s="7"/>
       <c r="I52" s="7"/>
     </row>
-    <row r="53" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>2584</v>
+        <v>2581</v>
       </c>
       <c r="B53" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="C53" s="7"/>
+      <c r="C53" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="D53" s="7" t="s">
-        <v>2557</v>
+        <v>2558</v>
       </c>
       <c r="E53" s="7"/>
-      <c r="F53" s="7" t="s">
-        <v>2553</v>
-      </c>
-      <c r="G53" s="9" t="s">
-        <v>2637</v>
-      </c>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>2585</v>
+        <v>2582</v>
       </c>
       <c r="B54" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="C54" s="7" t="s">
-        <v>2652</v>
-      </c>
+      <c r="C54" s="7"/>
       <c r="D54" s="7" t="s">
         <v>2556</v>
       </c>
-      <c r="E54" s="7" t="s">
-        <v>2564</v>
-      </c>
-      <c r="F54" s="7"/>
-      <c r="G54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7" t="s">
+        <v>2552</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>2630</v>
+      </c>
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>2586</v>
+        <v>2583</v>
       </c>
       <c r="B55" s="7" t="b">
         <v>0</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>2638</v>
+        <v>2644</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>2559</v>
-      </c>
-      <c r="E55" s="7"/>
+        <v>2555</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>2562</v>
+      </c>
       <c r="F55" s="7"/>
       <c r="G55" s="7"/>
       <c r="H55" s="7"/>
@@ -58065,188 +58069,192 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>2544</v>
+        <v>2584</v>
       </c>
       <c r="B56" s="7" t="b">
         <v>0</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>2652</v>
+        <v>2631</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>2556</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>2564</v>
-      </c>
+        <v>2558</v>
+      </c>
+      <c r="E56" s="7"/>
       <c r="F56" s="7"/>
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
     </row>
-    <row r="57" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>2587</v>
+        <v>2544</v>
       </c>
       <c r="B57" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="C57" s="7"/>
+      <c r="C57" s="7" t="s">
+        <v>2644</v>
+      </c>
       <c r="D57" s="7" t="s">
-        <v>2559</v>
-      </c>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7" t="s">
-        <v>2553</v>
-      </c>
-      <c r="G57" s="9" t="s">
-        <v>2639</v>
-      </c>
+        <v>2555</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>2562</v>
+      </c>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
     </row>
-    <row r="58" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>2588</v>
+        <v>2585</v>
       </c>
       <c r="B58" s="7" t="b">
         <v>0</v>
       </c>
       <c r="C58" s="7"/>
       <c r="D58" s="7" t="s">
-        <v>2651</v>
+        <v>2558</v>
       </c>
       <c r="E58" s="7"/>
       <c r="F58" s="7" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="G58" s="9" t="s">
-        <v>2641</v>
+        <v>2632</v>
       </c>
       <c r="H58" s="7"/>
       <c r="I58" s="7"/>
     </row>
-    <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>2589</v>
+        <v>2586</v>
       </c>
       <c r="B59" s="7" t="b">
         <v>0</v>
       </c>
       <c r="C59" s="7"/>
       <c r="D59" s="7" t="s">
-        <v>2559</v>
+        <v>2643</v>
       </c>
       <c r="E59" s="7"/>
       <c r="F59" s="7" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>2640</v>
+        <v>2634</v>
       </c>
       <c r="H59" s="7"/>
       <c r="I59" s="7"/>
     </row>
-    <row r="60" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>2590</v>
+        <v>2587</v>
       </c>
       <c r="B60" s="7" t="b">
         <v>0</v>
       </c>
       <c r="C60" s="7"/>
       <c r="D60" s="7" t="s">
-        <v>2556</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>2564</v>
-      </c>
+        <v>2558</v>
+      </c>
+      <c r="E60" s="7"/>
       <c r="F60" s="7" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>2642</v>
+        <v>2633</v>
       </c>
       <c r="H60" s="7"/>
       <c r="I60" s="7"/>
     </row>
-    <row r="61" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>2591</v>
+        <v>2588</v>
       </c>
       <c r="B61" s="7" t="b">
         <v>0</v>
       </c>
       <c r="C61" s="7"/>
       <c r="D61" s="7" t="s">
-        <v>2559</v>
-      </c>
-      <c r="E61" s="7"/>
+        <v>2555</v>
+      </c>
+      <c r="E61" s="7" t="s">
+        <v>2562</v>
+      </c>
       <c r="F61" s="7" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="G61" s="9" t="s">
-        <v>2643</v>
+        <v>2635</v>
       </c>
       <c r="H61" s="7"/>
       <c r="I61" s="7"/>
     </row>
-    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>2592</v>
+        <v>2589</v>
       </c>
       <c r="B62" s="7" t="b">
         <v>0</v>
       </c>
       <c r="C62" s="7"/>
       <c r="D62" s="7" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
       <c r="E62" s="7"/>
       <c r="F62" s="7" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="G62" s="9" t="s">
-        <v>2644</v>
+        <v>2636</v>
       </c>
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
     </row>
-    <row r="63" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>2593</v>
+        <v>2590</v>
       </c>
       <c r="B63" s="7" t="b">
         <v>0</v>
       </c>
       <c r="C63" s="7"/>
       <c r="D63" s="7" t="s">
-        <v>2557</v>
+        <v>2558</v>
       </c>
       <c r="E63" s="7"/>
       <c r="F63" s="7" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="G63" s="9" t="s">
-        <v>2645</v>
+        <v>2637</v>
       </c>
       <c r="H63" s="7"/>
       <c r="I63" s="7"/>
     </row>
-    <row r="64" spans="1:9" s="6" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="7"/>
-      <c r="B64" s="7"/>
+    <row r="64" spans="1:9" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
+        <v>2591</v>
+      </c>
+      <c r="B64" s="7" t="b">
+        <v>0</v>
+      </c>
       <c r="C64" s="7"/>
-      <c r="D64" s="7"/>
+      <c r="D64" s="7" t="s">
+        <v>2556</v>
+      </c>
       <c r="E64" s="7"/>
-      <c r="F64" s="7"/>
-      <c r="G64" s="9"/>
-      <c r="H64" s="7" t="s">
-        <v>2646</v>
-      </c>
-      <c r="I64" s="7">
-        <v>487</v>
-      </c>
+      <c r="F64" s="7" t="s">
+        <v>2552</v>
+      </c>
+      <c r="G64" s="9" t="s">
+        <v>2638</v>
+      </c>
+      <c r="H64" s="7"/>
+      <c r="I64" s="7"/>
     </row>
     <row r="65" spans="1:9" s="6" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7"/>
@@ -58257,10 +58265,10 @@
       <c r="F65" s="7"/>
       <c r="G65" s="9"/>
       <c r="H65" s="7" t="s">
-        <v>2647</v>
+        <v>2639</v>
       </c>
       <c r="I65" s="7">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="66" spans="1:9" s="6" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -58272,10 +58280,10 @@
       <c r="F66" s="7"/>
       <c r="G66" s="9"/>
       <c r="H66" s="7" t="s">
-        <v>2648</v>
+        <v>2640</v>
       </c>
       <c r="I66" s="7">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="67" spans="1:9" s="6" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -58287,10 +58295,10 @@
       <c r="F67" s="7"/>
       <c r="G67" s="9"/>
       <c r="H67" s="7" t="s">
-        <v>2649</v>
+        <v>2641</v>
       </c>
       <c r="I67" s="7">
-        <v>485</v>
+        <v>488</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="6" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -58301,33 +58309,29 @@
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
       <c r="G68" s="9"/>
-      <c r="H68" s="7"/>
+      <c r="H68" s="7" t="s">
+        <v>2642</v>
+      </c>
       <c r="I68" s="7">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
-        <v>2594</v>
-      </c>
-      <c r="B69" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="C69" s="7">
-        <v>0</v>
-      </c>
-      <c r="D69" s="7" t="s">
-        <v>2557</v>
-      </c>
+        <v>485</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" s="6" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="7"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="7"/>
       <c r="E69" s="7"/>
       <c r="F69" s="7"/>
-      <c r="G69" s="7"/>
+      <c r="G69" s="9"/>
       <c r="H69" s="7"/>
-      <c r="I69" s="7"/>
+      <c r="I69" s="7">
+        <v>-3</v>
+      </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>2595</v>
+        <v>2592</v>
       </c>
       <c r="B70" s="7" t="b">
         <v>0</v>
@@ -58336,7 +58340,7 @@
         <v>0</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>2559</v>
+        <v>2556</v>
       </c>
       <c r="E70" s="7"/>
       <c r="F70" s="7"/>
@@ -58346,7 +58350,7 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>2596</v>
+        <v>2593</v>
       </c>
       <c r="B71" s="7" t="b">
         <v>0</v>
@@ -58355,7 +58359,7 @@
         <v>0</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
       <c r="E71" s="7"/>
       <c r="F71" s="7"/>
@@ -58365,7 +58369,7 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>2597</v>
+        <v>2594</v>
       </c>
       <c r="B72" s="7" t="b">
         <v>0</v>
@@ -58374,7 +58378,7 @@
         <v>0</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>2557</v>
+        <v>2558</v>
       </c>
       <c r="E72" s="7"/>
       <c r="F72" s="7"/>
@@ -58384,7 +58388,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>2598</v>
+        <v>2595</v>
       </c>
       <c r="B73" s="7" t="b">
         <v>0</v>
@@ -58393,7 +58397,7 @@
         <v>0</v>
       </c>
       <c r="D73" s="7" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="E73" s="7"/>
       <c r="F73" s="7"/>
@@ -58403,7 +58407,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>2599</v>
+        <v>2596</v>
       </c>
       <c r="B74" s="7" t="b">
         <v>0</v>
@@ -58412,7 +58416,7 @@
         <v>0</v>
       </c>
       <c r="D74" s="7" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="E74" s="7"/>
       <c r="F74" s="7"/>
@@ -58420,45 +58424,64 @@
       <c r="H74" s="7"/>
       <c r="I74" s="7"/>
     </row>
-    <row r="75" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>2600</v>
+        <v>2597</v>
       </c>
       <c r="B75" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="C75" s="7"/>
+      <c r="C75" s="7">
+        <v>0</v>
+      </c>
       <c r="D75" s="7" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="E75" s="7"/>
-      <c r="F75" s="7" t="s">
-        <v>2553</v>
-      </c>
-      <c r="G75" s="9" t="s">
-        <v>2650</v>
-      </c>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>2601</v>
+        <v>2598</v>
       </c>
       <c r="B76" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="C76" s="7">
-        <v>0</v>
-      </c>
+      <c r="C76" s="7"/>
       <c r="D76" s="7" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="E76" s="7"/>
-      <c r="F76" s="7"/>
-      <c r="G76" s="9"/>
+      <c r="F76" s="7" t="s">
+        <v>2552</v>
+      </c>
+      <c r="G76" s="9" t="s">
+        <v>2653</v>
+      </c>
       <c r="H76" s="7"/>
       <c r="I76" s="7"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
+        <v>2599</v>
+      </c>
+      <c r="B77" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="C77" s="7">
+        <v>0</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>2556</v>
+      </c>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="7"/>
+      <c r="I77" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -58476,13 +58499,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>304800</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -58498,13 +58521,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>304800</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -58520,13 +58543,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>304800</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -58542,13 +58565,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>304800</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -58564,13 +58587,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>304800</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -58586,13 +58609,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>304800</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -58608,13 +58631,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>304800</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -58630,13 +58653,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>304800</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -58652,13 +58675,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>304800</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -58674,13 +58697,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>304800</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -58696,13 +58719,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>304800</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -58718,13 +58741,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>304800</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -58740,13 +58763,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>304800</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -58762,13 +58785,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>304800</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -58784,13 +58807,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>304800</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -58806,13 +58829,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>304800</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -58828,13 +58851,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>304800</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -58850,13 +58873,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>304800</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -58872,13 +58895,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>304800</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -58894,13 +58917,13 @@
                   <from>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>20</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>304800</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>21</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -58918,13 +58941,13 @@
           <x14:formula1>
             <xm:f>lookups!$B$2:$B$23</xm:f>
           </x14:formula1>
-          <xm:sqref>C3 D5:D76</xm:sqref>
+          <xm:sqref>C3:C4 D6:D77</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>lookups!$A$2:$A$23</xm:f>
           </x14:formula1>
-          <xm:sqref>F5:F76</xm:sqref>
+          <xm:sqref>F6:F77</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -58936,7 +58959,7 @@
           <x14:formula1>
             <xm:f>lookups!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B5:B76</xm:sqref>
+          <xm:sqref>B6:B77</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -58961,21 +58984,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>2549</v>
+        <v>2548</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>2555</v>
+        <v>2554</v>
       </c>
       <c r="C1" t="s">
-        <v>2565</v>
+        <v>2563</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2552</v>
+        <v>2551</v>
       </c>
       <c r="B2" t="s">
-        <v>2556</v>
+        <v>2555</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
@@ -58983,10 +59006,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="B3" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="C3" t="b">
         <v>0</v>
@@ -58994,20 +59017,20 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2554</v>
+        <v>2553</v>
       </c>
       <c r="B4" t="s">
-        <v>2558</v>
+        <v>2557</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>2651</v>
+        <v>2643</v>
       </c>
     </row>
   </sheetData>

</xml_diff>